<commit_message>
Highlight cells with task names which already mentioned in YT as solved in this repository
</commit_message>
<xml_diff>
--- a/interview-materials/Yandex Interview Kit.xlsx
+++ b/interview-materials/Yandex Interview Kit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\personal\java-interview-coding\interview-materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4511ABA-2460-4728-995F-12B4CAAA9B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C48D135-67C6-431B-A73A-D41F252ABBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -309,7 +309,7 @@
       <name val="-apple-system"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,6 +346,12 @@
         <bgColor rgb="FFD9534F"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -374,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -419,6 +425,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,16 +647,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="74.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -659,12 +671,15 @@
       <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="14.25">
+      <c r="F1" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.25">
       <c r="A2" s="1">
         <v>771</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="16" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="3">
@@ -674,7 +689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.25">
+    <row r="3" spans="1:6" ht="14.25">
       <c r="A3" s="5">
         <v>938</v>
       </c>
@@ -688,7 +703,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.25">
+    <row r="4" spans="1:6" ht="14.25">
       <c r="A4" s="1">
         <v>763</v>
       </c>
@@ -702,7 +717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.25">
+    <row r="5" spans="1:6" ht="14.25">
       <c r="A5" s="1">
         <v>1650</v>
       </c>
@@ -716,7 +731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.25">
+    <row r="6" spans="1:6" ht="14.25">
       <c r="A6" s="1">
         <v>557</v>
       </c>
@@ -730,7 +745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.25">
+    <row r="7" spans="1:6" ht="14.25">
       <c r="A7" s="1">
         <v>933</v>
       </c>
@@ -744,11 +759,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.25">
+    <row r="8" spans="1:6" ht="14.25">
       <c r="A8" s="1">
         <v>977</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="16" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="3">
@@ -758,7 +773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.25">
+    <row r="9" spans="1:6" ht="14.25">
       <c r="A9" s="5">
         <v>986</v>
       </c>
@@ -772,7 +787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.25">
+    <row r="10" spans="1:6" ht="14.25">
       <c r="A10" s="11">
         <v>136</v>
       </c>
@@ -786,35 +801,35 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.25">
-      <c r="A11" s="5">
+    <row r="11" spans="1:6" ht="14.25">
+      <c r="A11" s="1">
+        <v>22</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="14.25">
+      <c r="A12" s="5">
         <v>206</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C12" s="7">
         <v>0.69199999999999995</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="14.25">
-      <c r="A12" s="1">
-        <v>22</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0.69199999999999995</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="14.25">
+      <c r="D12" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="14.25">
       <c r="A13" s="1">
         <v>362</v>
       </c>
@@ -828,7 +843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.25">
+    <row r="14" spans="1:6" ht="14.25">
       <c r="A14" s="5">
         <v>238</v>
       </c>
@@ -842,7 +857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.25">
+    <row r="15" spans="1:6" ht="14.25">
       <c r="A15" s="5">
         <v>49</v>
       </c>
@@ -856,7 +871,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.25">
+    <row r="16" spans="1:6" ht="14.25">
       <c r="A16" s="1">
         <v>1004</v>
       </c>
@@ -888,7 +903,7 @@
       <c r="A18" s="8">
         <v>283</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="9">
@@ -944,7 +959,7 @@
       <c r="A22" s="5">
         <v>268</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="16" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="7">
@@ -972,7 +987,7 @@
       <c r="A24" s="5">
         <v>341</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="16" t="s">
         <v>38</v>
       </c>
       <c r="C24" s="7">
@@ -1014,7 +1029,7 @@
       <c r="A27" s="1">
         <v>42</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="16" t="s">
         <v>29</v>
       </c>
       <c r="C27" s="3">
@@ -1140,7 +1155,7 @@
       <c r="A36" s="5">
         <v>101</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C36" s="7">
@@ -1196,7 +1211,7 @@
       <c r="A40" s="5">
         <v>1</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C40" s="7">
@@ -1210,7 +1225,7 @@
       <c r="A41" s="5">
         <v>26</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="16" t="s">
         <v>64</v>
       </c>
       <c r="C41" s="7">
@@ -1238,7 +1253,7 @@
       <c r="A43" s="5">
         <v>849</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C43" s="7">
@@ -1266,7 +1281,7 @@
       <c r="A45" s="5">
         <v>443</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C45" s="7">
@@ -1448,7 +1463,7 @@
       <c r="A58" s="5">
         <v>125</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C58" s="7">
@@ -1462,7 +1477,7 @@
       <c r="A59" s="5">
         <v>20</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C59" s="7">
@@ -1476,7 +1491,7 @@
       <c r="A60" s="5">
         <v>146</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C60" s="7">
@@ -1490,7 +1505,7 @@
       <c r="A61" s="5">
         <v>19</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="16" t="s">
         <v>56</v>
       </c>
       <c r="C61" s="7">
@@ -1546,7 +1561,7 @@
       <c r="A65" s="1">
         <v>71</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="16" t="s">
         <v>53</v>
       </c>
       <c r="C65" s="3">
@@ -1602,7 +1617,7 @@
       <c r="A69" s="1">
         <v>3</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C69" s="3">
@@ -1630,7 +1645,7 @@
       <c r="A71" s="5">
         <v>98</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C71" s="7">
@@ -1681,10 +1696,10 @@
     <hyperlink ref="B35" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="A60" r:id="rId21" display="https://leetcode.com/problems/lru-cache" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
     <hyperlink ref="B60" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="A12" r:id="rId23" display="https://leetcode.com/problems/generate-parentheses" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B12" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A11" r:id="rId25" display="https://leetcode.com/problems/reverse-linked-list" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B11" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A11" r:id="rId23" display="https://leetcode.com/problems/generate-parentheses" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B11" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A12" r:id="rId25" display="https://leetcode.com/problems/reverse-linked-list" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B12" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="A52" r:id="rId27" display="https://leetcode.com/problems/permutation-in-string" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="B52" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
     <hyperlink ref="A47" r:id="rId29" display="https://leetcode.com/problems/merge-k-sorted-lists" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>

</xml_diff>

<commit_message>
Adjust Yandex Interview Kit: mark with color some solved tasks (30/71)
</commit_message>
<xml_diff>
--- a/interview-materials/Yandex Interview Kit.xlsx
+++ b/interview-materials/Yandex Interview Kit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\personal\java-interview-coding\interview-materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C48D135-67C6-431B-A73A-D41F252ABBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A41FE24-02E3-4A40-85B0-497B8EF95C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -429,6 +429,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,7 +652,7 @@
   </sheetPr>
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -672,7 +675,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="17">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25">
@@ -693,7 +696,7 @@
       <c r="A3" s="5">
         <v>938</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="16" t="s">
         <v>66</v>
       </c>
       <c r="C3" s="7">
@@ -705,125 +708,125 @@
     </row>
     <row r="4" spans="1:6" ht="14.25">
       <c r="A4" s="1">
-        <v>763</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>67</v>
+        <v>557</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="C4" s="3">
-        <v>0.78600000000000003</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>5</v>
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.25">
       <c r="A5" s="1">
-        <v>1650</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>59</v>
+        <v>933</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="C5" s="3">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>5</v>
+        <v>0.73</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.25">
       <c r="A6" s="1">
-        <v>557</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>71</v>
+        <v>977</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>55</v>
       </c>
       <c r="C6" s="3">
-        <v>0.77200000000000002</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.25">
-      <c r="A7" s="1">
-        <v>933</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.73</v>
+      <c r="A7" s="11">
+        <v>136</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.70199999999999996</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.25">
-      <c r="A8" s="1">
-        <v>977</v>
+      <c r="A8" s="5">
+        <v>206</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.71499999999999997</v>
+        <v>19</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.69199999999999995</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.25">
-      <c r="A9" s="5">
-        <v>986</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="7">
-        <v>0.70699999999999996</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>5</v>
+      <c r="A9" s="1">
+        <v>1446</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="14.25">
-      <c r="A10" s="11">
-        <v>136</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="12">
-        <v>0.70199999999999996</v>
+      <c r="A10" s="8">
+        <v>283</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.61399999999999999</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.25">
-      <c r="A11" s="1">
-        <v>22</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.69199999999999995</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>5</v>
+      <c r="A11" s="5">
+        <v>21</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.25">
       <c r="A12" s="5">
-        <v>206</v>
+        <v>268</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="C12" s="7">
-        <v>0.69199999999999995</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>8</v>
@@ -831,181 +834,181 @@
     </row>
     <row r="13" spans="1:6" ht="14.25">
       <c r="A13" s="1">
-        <v>362</v>
+        <v>167</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="C13" s="3">
-        <v>0.66900000000000004</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>5</v>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.25">
-      <c r="A14" s="5">
-        <v>238</v>
+      <c r="A14" s="1">
+        <v>232</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="7">
-        <v>0.63400000000000001</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>5</v>
+        <v>41</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.25">
       <c r="A15" s="5">
-        <v>49</v>
+        <v>387</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="C15" s="7">
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>5</v>
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="14.25">
       <c r="A16" s="1">
-        <v>1004</v>
+        <v>350</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C16" s="3">
-        <v>0.623</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>5</v>
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25">
-      <c r="A17" s="1">
-        <v>1446</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0.62</v>
+      <c r="A17" s="5">
+        <v>415</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.51500000000000001</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25">
-      <c r="A18" s="8">
-        <v>283</v>
+      <c r="A18" s="5">
+        <v>101</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="9">
-        <v>0.61399999999999999</v>
+        <v>34</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.50900000000000001</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25">
-      <c r="A19" s="1">
-        <v>281</v>
+      <c r="A19" s="5">
+        <v>392</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0.61</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>5</v>
+        <v>54</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.501</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25">
       <c r="A20" s="5">
-        <v>1493</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="C20" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>5</v>
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25">
       <c r="A21" s="5">
-        <v>21</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>44</v>
+        <v>26</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>64</v>
       </c>
       <c r="C21" s="7">
-        <v>0.59099999999999997</v>
+        <v>0.48099999999999998</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25">
-      <c r="A22" s="5">
-        <v>268</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="7">
-        <v>0.58499999999999996</v>
+      <c r="A22" s="1">
+        <v>234</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.45500000000000002</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25">
-      <c r="A23" s="1">
-        <v>167</v>
+      <c r="A23" s="5">
+        <v>716</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0.57999999999999996</v>
+        <v>58</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.44700000000000001</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25">
-      <c r="A24" s="5">
-        <v>341</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="7">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>5</v>
+      <c r="A24" s="1">
+        <v>228</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25">
       <c r="A25" s="1">
-        <v>232</v>
+        <v>88</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C25" s="3">
-        <v>0.56599999999999995</v>
+        <v>0.43</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>8</v>
@@ -1013,125 +1016,125 @@
     </row>
     <row r="26" spans="1:4" ht="14.25">
       <c r="A26" s="5">
-        <v>387</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>74</v>
+        <v>125</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>11</v>
       </c>
       <c r="C26" s="7">
-        <v>0.56399999999999995</v>
+        <v>0.40699999999999997</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25">
-      <c r="A27" s="1">
-        <v>42</v>
+      <c r="A27" s="5">
+        <v>20</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="3">
-        <v>0.55400000000000005</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25">
-      <c r="A28" s="8">
-        <v>103</v>
+      <c r="A28" s="1">
+        <v>763</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="9">
-        <v>0.55300000000000005</v>
-      </c>
-      <c r="D28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25">
       <c r="A29" s="1">
-        <v>350</v>
+        <v>1650</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C29" s="3">
-        <v>0.54400000000000004</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>8</v>
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25">
       <c r="A30" s="5">
-        <v>236</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>48</v>
+        <v>986</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="C30" s="7">
-        <v>0.54</v>
-      </c>
-      <c r="D30" s="4" t="s">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25">
       <c r="A31" s="1">
-        <v>200</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="C31" s="3">
-        <v>0.52900000000000003</v>
+        <v>0.69199999999999995</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25">
-      <c r="A32" s="5">
-        <v>159</v>
+      <c r="A32" s="1">
+        <v>362</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="7">
-        <v>0.52200000000000002</v>
-      </c>
-      <c r="D32" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25">
       <c r="A33" s="5">
-        <v>415</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>72</v>
+        <v>238</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>68</v>
       </c>
       <c r="C33" s="7">
-        <v>0.51500000000000001</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>8</v>
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25">
-      <c r="A34" s="1">
-        <v>279</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="3">
-        <v>0.51500000000000001</v>
+      <c r="A34" s="5">
+        <v>49</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="7">
+        <v>0.63200000000000001</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>5</v>
@@ -1139,69 +1142,69 @@
     </row>
     <row r="35" spans="1:4" ht="14.25">
       <c r="A35" s="1">
-        <v>380</v>
+        <v>1004</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C35" s="3">
-        <v>0.51</v>
+        <v>0.623</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25">
-      <c r="A36" s="5">
-        <v>101</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="7">
-        <v>0.50900000000000001</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>8</v>
+      <c r="A36" s="1">
+        <v>281</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="14.25">
       <c r="A37" s="5">
-        <v>392</v>
+        <v>1493</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="C37" s="7">
-        <v>0.501</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>8</v>
+        <v>0.6</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.25">
-      <c r="A38" s="1">
-        <v>253</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="3">
-        <v>0.49099999999999999</v>
-      </c>
-      <c r="D38" s="4" t="s">
+      <c r="A38" s="5">
+        <v>341</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="14.25">
-      <c r="A39" s="1">
-        <v>487</v>
+      <c r="A39" s="8">
+        <v>103</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="3">
-        <v>0.48599999999999999</v>
+        <v>75</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0.55300000000000005</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>5</v>
@@ -1209,83 +1212,83 @@
     </row>
     <row r="40" spans="1:4" ht="14.25">
       <c r="A40" s="5">
-        <v>1</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>30</v>
+        <v>236</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="C40" s="7">
-        <v>0.48199999999999998</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>8</v>
+        <v>0.54</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="14.25">
-      <c r="A41" s="5">
-        <v>26</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="7">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>8</v>
+      <c r="A41" s="1">
+        <v>200</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14.25">
-      <c r="A42" s="1">
-        <v>153</v>
+      <c r="A42" s="5">
+        <v>159</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="3">
-        <v>0.47599999999999998</v>
+        <v>60</v>
+      </c>
+      <c r="C42" s="7">
+        <v>0.52200000000000002</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="14.25">
-      <c r="A43" s="5">
-        <v>849</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="7">
-        <v>0.47399999999999998</v>
+      <c r="A43" s="1">
+        <v>279</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0.51500000000000001</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="14.25">
-      <c r="A44" s="5">
-        <v>438</v>
+      <c r="A44" s="1">
+        <v>380</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" s="7">
-        <v>0.47099999999999997</v>
+        <v>16</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0.51</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="14.25">
-      <c r="A45" s="5">
-        <v>443</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="7">
-        <v>0.46899999999999997</v>
+      <c r="A45" s="1">
+        <v>253</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0.49099999999999999</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>5</v>
@@ -1293,293 +1296,293 @@
     </row>
     <row r="46" spans="1:4" ht="14.25">
       <c r="A46" s="1">
+        <v>487</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="14.25">
+      <c r="A47" s="1">
+        <v>153</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A48" s="5">
+        <v>849</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="7">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A49" s="5">
+        <v>438</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="7">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A50" s="5">
+        <v>443</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="7">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A51" s="1">
         <v>470</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B51" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C51" s="3">
         <v>0.46600000000000003</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="14.25">
-      <c r="A47" s="5">
-        <v>23</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C47" s="7">
-        <v>0.45800000000000002</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="14.25">
-      <c r="A48" s="1">
-        <v>234</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C48" s="3">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="14.25">
-      <c r="A49" s="5">
-        <v>716</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C49" s="7">
-        <v>0.44700000000000001</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="14.25">
-      <c r="A50" s="1">
-        <v>228</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" s="3">
-        <v>0.44500000000000001</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="14.25">
-      <c r="A51" s="5">
+      <c r="D51" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A52" s="5">
         <v>56</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B52" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C52" s="7">
         <v>0.442</v>
       </c>
-      <c r="D51" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="14.25">
-      <c r="A52" s="1">
+      <c r="D52" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A53" s="1">
         <v>567</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B53" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C53" s="3">
         <v>0.441</v>
       </c>
-      <c r="D52" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="14.25">
-      <c r="A53" s="5">
+      <c r="D53" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A54" s="5">
         <v>560</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B54" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C54" s="7">
         <v>0.438</v>
       </c>
-      <c r="D53" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A54" s="1">
-        <v>88</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" s="3">
-        <v>0.43</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>8</v>
+      <c r="D54" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1">
       <c r="A55" s="1">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C55" s="3">
-        <v>0.42099999999999999</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>22</v>
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A56" s="1">
-        <v>150</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C56" s="3">
-        <v>0.41399999999999998</v>
+      <c r="A56" s="5">
+        <v>146</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="7">
+        <v>0.39100000000000001</v>
       </c>
       <c r="D56" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A57" s="11">
-        <v>76</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C57" s="12">
-        <v>0.40799999999999997</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>22</v>
+      <c r="A57" s="5">
+        <v>19</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="7">
+        <v>0.377</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1">
       <c r="A58" s="5">
-        <v>125</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C58" s="7">
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>8</v>
+        <v>0.377</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1">
       <c r="A59" s="5">
-        <v>20</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C59" s="7">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>8</v>
+        <v>0.373</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A60" s="5">
-        <v>146</v>
+      <c r="A60" s="1">
+        <v>71</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C60" s="7">
-        <v>0.39100000000000001</v>
+        <v>53</v>
+      </c>
+      <c r="C60" s="3">
+        <v>0.372</v>
       </c>
       <c r="D60" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A61" s="5">
-        <v>19</v>
-      </c>
-      <c r="B61" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C61" s="7">
-        <v>0.377</v>
+      <c r="A61" s="1">
+        <v>356</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" s="3">
+        <v>0.34200000000000003</v>
       </c>
       <c r="D61" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A62" s="5">
-        <v>2</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C62" s="7">
-        <v>0.377</v>
+      <c r="A62" s="1">
+        <v>161</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" s="3">
+        <v>0.33800000000000002</v>
       </c>
       <c r="D62" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A63" s="5">
-        <v>33</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C63" s="7">
-        <v>0.373</v>
+      <c r="A63" s="1">
+        <v>3</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C63" s="3">
+        <v>0.32700000000000001</v>
       </c>
       <c r="D63" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A64" s="1">
-        <v>124</v>
+      <c r="A64" s="5">
+        <v>5</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C64" s="3">
-        <v>0.372</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>22</v>
+        <v>46</v>
+      </c>
+      <c r="C64" s="7">
+        <v>0.316</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A65" s="1">
-        <v>71</v>
+      <c r="A65" s="5">
+        <v>98</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C65" s="3">
-        <v>0.372</v>
+        <v>36</v>
+      </c>
+      <c r="C65" s="7">
+        <v>0.30099999999999999</v>
       </c>
       <c r="D65" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A66" s="1">
-        <v>356</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" s="3">
-        <v>0.34200000000000003</v>
+      <c r="A66" s="5">
+        <v>523</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" s="7">
+        <v>0.26700000000000002</v>
       </c>
       <c r="D66" s="10" t="s">
         <v>5</v>
@@ -1587,27 +1590,27 @@
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1">
       <c r="A67" s="1">
-        <v>161</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>12</v>
+        <v>42</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="C67" s="3">
-        <v>0.33800000000000002</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>5</v>
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1">
       <c r="A68" s="5">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="C68" s="7">
-        <v>0.33500000000000002</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="D68" s="14" t="s">
         <v>22</v>
@@ -1615,203 +1618,203 @@
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1">
       <c r="A69" s="1">
-        <v>3</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>35</v>
+        <v>85</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C69" s="3">
-        <v>0.32700000000000001</v>
-      </c>
-      <c r="D69" s="10" t="s">
-        <v>5</v>
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A70" s="5">
-        <v>5</v>
+      <c r="A70" s="11">
+        <v>76</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C70" s="7">
-        <v>0.316</v>
-      </c>
-      <c r="D70" s="10" t="s">
-        <v>5</v>
+        <v>76</v>
+      </c>
+      <c r="C70" s="12">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A71" s="5">
-        <v>98</v>
-      </c>
-      <c r="B71" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C71" s="7">
-        <v>0.30099999999999999</v>
-      </c>
-      <c r="D71" s="10" t="s">
-        <v>5</v>
+      <c r="A71" s="1">
+        <v>124</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C71" s="3">
+        <v>0.372</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1">
       <c r="A72" s="5">
-        <v>523</v>
+        <v>4</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C72" s="7">
-        <v>0.26700000000000002</v>
-      </c>
-      <c r="D72" s="10" t="s">
-        <v>5</v>
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D73">
-    <sortCondition descending="1" ref="C1:C73"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D66">
+    <sortCondition ref="D2:D66"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A66" r:id="rId1" display="https://leetcode.com/problems/line-reflection" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B66" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A20" r:id="rId3" display="https://leetcode.com/problems/longest-subarray-of-1s-after-deleting-one-element" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B20" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A50" r:id="rId5" display="https://leetcode.com/problems/summary-ranges" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B50" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="A45" r:id="rId7" display="https://leetcode.com/problems/string-compression" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B45" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="A19" r:id="rId9" display="https://leetcode.com/problems/zigzag-iterator" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B19" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="A58" r:id="rId11" display="https://leetcode.com/problems/valid-palindrome" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B58" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="A67" r:id="rId13" display="https://leetcode.com/problems/one-edit-distance" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B67" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="A53" r:id="rId15" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B53" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="A15" r:id="rId17" display="https://leetcode.com/problems/group-anagrams" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B15" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="A35" r:id="rId19" display="https://leetcode.com/problems/insert-delete-getrandom-o1" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B35" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="A60" r:id="rId21" display="https://leetcode.com/problems/lru-cache" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B60" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="A11" r:id="rId23" display="https://leetcode.com/problems/generate-parentheses" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B11" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A12" r:id="rId25" display="https://leetcode.com/problems/reverse-linked-list" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B12" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="A52" r:id="rId27" display="https://leetcode.com/problems/permutation-in-string" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B52" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="A47" r:id="rId29" display="https://leetcode.com/problems/merge-k-sorted-lists" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B47" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="A7" r:id="rId31" display="https://leetcode.com/problems/number-of-recent-calls" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B7" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="A59" r:id="rId33" display="https://leetcode.com/problems/valid-parentheses" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="B59" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="A39" r:id="rId35" display="https://leetcode.com/problems/max-consecutive-ones-ii" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B39" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="A43" r:id="rId37" display="https://leetcode.com/problems/maximize-distance-to-closest-person" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B43" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="A13" r:id="rId39" display="https://leetcode.com/problems/design-hit-counter" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B13" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="A51" r:id="rId41" display="https://leetcode.com/problems/merge-intervals" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B51" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="A27" r:id="rId43" display="https://leetcode.com/problems/trapping-rain-water" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B27" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="A40" r:id="rId45" display="https://leetcode.com/problems/two-sum" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="B40" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="A38" r:id="rId47" display="https://leetcode.com/problems/meeting-rooms-ii" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="B38" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="A44" r:id="rId49" display="https://leetcode.com/problems/find-all-anagrams-in-a-string" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B44" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="A46" r:id="rId51" display="https://leetcode.com/problems/implement-rand10-using-rand7" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B46" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="A36" r:id="rId53" display="https://leetcode.com/problems/symmetric-tree" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="B36" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="A69" r:id="rId55" display="https://leetcode.com/problems/longest-substring-without-repeating-characters" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B69" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="A71" r:id="rId57" display="https://leetcode.com/problems/validate-binary-search-tree" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="B71" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="A31" r:id="rId59" display="https://leetcode.com/problems/number-of-islands" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B31" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="A24" r:id="rId61" display="https://leetcode.com/problems/flatten-nested-list-iterator" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B24" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="A17" r:id="rId63" display="https://leetcode.com/problems/consecutive-characters" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="B17" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="A9" r:id="rId65" display="https://leetcode.com/problems/interval-list-intersections" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="B9" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="A25" r:id="rId67" display="https://leetcode.com/problems/implement-queue-using-stacks" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="B25" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="A62" r:id="rId69" display="https://leetcode.com/problems/add-two-numbers" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="B62" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="A54" r:id="rId71" display="https://leetcode.com/problems/merge-sorted-array" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="B54" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="A21" r:id="rId73" display="https://leetcode.com/problems/merge-two-sorted-lists" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="B21" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="A16" r:id="rId75" display="https://leetcode.com/problems/max-consecutive-ones-iii" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="B16" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="A70" r:id="rId77" display="https://leetcode.com/problems/longest-palindromic-substring" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="B70" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="A61" r:id="rId1" display="https://leetcode.com/problems/line-reflection" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B61" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A37" r:id="rId3" display="https://leetcode.com/problems/longest-subarray-of-1s-after-deleting-one-element" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B37" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A24" r:id="rId5" display="https://leetcode.com/problems/summary-ranges" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B24" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A50" r:id="rId7" display="https://leetcode.com/problems/string-compression" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B50" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A36" r:id="rId9" display="https://leetcode.com/problems/zigzag-iterator" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B36" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A26" r:id="rId11" display="https://leetcode.com/problems/valid-palindrome" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B26" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A62" r:id="rId13" display="https://leetcode.com/problems/one-edit-distance" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B62" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A54" r:id="rId15" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B54" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A34" r:id="rId17" display="https://leetcode.com/problems/group-anagrams" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B34" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A44" r:id="rId19" display="https://leetcode.com/problems/insert-delete-getrandom-o1" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B44" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A56" r:id="rId21" display="https://leetcode.com/problems/lru-cache" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B56" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A31" r:id="rId23" display="https://leetcode.com/problems/generate-parentheses" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B31" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A8" r:id="rId25" display="https://leetcode.com/problems/reverse-linked-list" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B8" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A53" r:id="rId27" display="https://leetcode.com/problems/permutation-in-string" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B53" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="A68" r:id="rId29" display="https://leetcode.com/problems/merge-k-sorted-lists" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B68" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="A5" r:id="rId31" display="https://leetcode.com/problems/number-of-recent-calls" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B5" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="A27" r:id="rId33" display="https://leetcode.com/problems/valid-parentheses" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B27" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="A46" r:id="rId35" display="https://leetcode.com/problems/max-consecutive-ones-ii" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B46" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="A48" r:id="rId37" display="https://leetcode.com/problems/maximize-distance-to-closest-person" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B48" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="A32" r:id="rId39" display="https://leetcode.com/problems/design-hit-counter" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B32" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="A52" r:id="rId41" display="https://leetcode.com/problems/merge-intervals" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B52" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="A67" r:id="rId43" display="https://leetcode.com/problems/trapping-rain-water" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B67" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="A20" r:id="rId45" display="https://leetcode.com/problems/two-sum" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B20" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="A45" r:id="rId47" display="https://leetcode.com/problems/meeting-rooms-ii" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B45" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="A49" r:id="rId49" display="https://leetcode.com/problems/find-all-anagrams-in-a-string" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B49" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="A51" r:id="rId51" display="https://leetcode.com/problems/implement-rand10-using-rand7" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B51" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="A18" r:id="rId53" display="https://leetcode.com/problems/symmetric-tree" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B18" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="A63" r:id="rId55" display="https://leetcode.com/problems/longest-substring-without-repeating-characters" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B63" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="A65" r:id="rId57" display="https://leetcode.com/problems/validate-binary-search-tree" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B65" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="A41" r:id="rId59" display="https://leetcode.com/problems/number-of-islands" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B41" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="A38" r:id="rId61" display="https://leetcode.com/problems/flatten-nested-list-iterator" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B38" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="A9" r:id="rId63" display="https://leetcode.com/problems/consecutive-characters" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B9" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="A30" r:id="rId65" display="https://leetcode.com/problems/interval-list-intersections" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B30" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="A14" r:id="rId67" display="https://leetcode.com/problems/implement-queue-using-stacks" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B14" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="A58" r:id="rId69" display="https://leetcode.com/problems/add-two-numbers" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B58" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="A25" r:id="rId71" display="https://leetcode.com/problems/merge-sorted-array" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B25" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="A11" r:id="rId73" display="https://leetcode.com/problems/merge-two-sorted-lists" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B11" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="A35" r:id="rId75" display="https://leetcode.com/problems/max-consecutive-ones-iii" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B35" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="A64" r:id="rId77" display="https://leetcode.com/problems/longest-palindromic-substring" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B64" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
     <hyperlink ref="A2" r:id="rId79" display="https://leetcode.com/problems/jewels-and-stones" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
     <hyperlink ref="B2" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="A30" r:id="rId81" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-tree" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="B30" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="A29" r:id="rId83" display="https://leetcode.com/problems/intersection-of-two-arrays-ii" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="B29" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="A22" r:id="rId85" display="https://leetcode.com/problems/missing-number" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="B22" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="A56" r:id="rId87" display="https://leetcode.com/problems/evaluate-reverse-polish-notation" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="B56" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="A68" r:id="rId89" display="https://leetcode.com/problems/median-of-two-sorted-arrays" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="B68" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="A65" r:id="rId91" display="https://leetcode.com/problems/simplify-path" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="B65" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="A37" r:id="rId93" display="https://leetcode.com/problems/is-subsequence" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="B37" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="A8" r:id="rId95" display="https://leetcode.com/problems/squares-of-a-sorted-array" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="B8" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="A61" r:id="rId97" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="B61" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="A34" r:id="rId99" display="https://leetcode.com/problems/perfect-squares" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="B34" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="A49" r:id="rId101" display="https://leetcode.com/problems/max-stack" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="B49" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="A5" r:id="rId103" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-tree-iii" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="B5" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="A32" r:id="rId105" display="https://leetcode.com/problems/longest-substring-with-at-most-two-distinct-characters" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="B32" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="A55" r:id="rId107" display="https://leetcode.com/problems/maximal-rectangle" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="B55" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="A63" r:id="rId109" display="https://leetcode.com/problems/search-in-rotated-sorted-array" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="B63" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="A23" r:id="rId111" display="https://leetcode.com/problems/two-sum-ii-input-array-is-sorted" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="B23" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="A41" r:id="rId113" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="B41" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="A42" r:id="rId115" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="B42" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="A40" r:id="rId81" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-tree" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B40" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="A16" r:id="rId83" display="https://leetcode.com/problems/intersection-of-two-arrays-ii" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B16" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="A12" r:id="rId85" display="https://leetcode.com/problems/missing-number" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B12" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="A55" r:id="rId87" display="https://leetcode.com/problems/evaluate-reverse-polish-notation" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B55" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="A72" r:id="rId89" display="https://leetcode.com/problems/median-of-two-sorted-arrays" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B72" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="A60" r:id="rId91" display="https://leetcode.com/problems/simplify-path" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B60" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="A19" r:id="rId93" display="https://leetcode.com/problems/is-subsequence" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B19" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="A6" r:id="rId95" display="https://leetcode.com/problems/squares-of-a-sorted-array" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B6" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="A57" r:id="rId97" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B57" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="A43" r:id="rId99" display="https://leetcode.com/problems/perfect-squares" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="B43" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="A23" r:id="rId101" display="https://leetcode.com/problems/max-stack" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="B23" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="A29" r:id="rId103" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-tree-iii" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="B29" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="A42" r:id="rId105" display="https://leetcode.com/problems/longest-substring-with-at-most-two-distinct-characters" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="B42" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="A69" r:id="rId107" display="https://leetcode.com/problems/maximal-rectangle" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="B69" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="A59" r:id="rId109" display="https://leetcode.com/problems/search-in-rotated-sorted-array" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="B59" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="A13" r:id="rId111" display="https://leetcode.com/problems/two-sum-ii-input-array-is-sorted" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="B13" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="A21" r:id="rId113" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="B21" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="A47" r:id="rId115" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="B47" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
     <hyperlink ref="A3" r:id="rId117" display="https://leetcode.com/problems/range-sum-of-bst" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
     <hyperlink ref="B3" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="A4" r:id="rId119" display="https://leetcode.com/problems/partition-labels" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="B4" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="A14" r:id="rId121" display="https://leetcode.com/problems/product-of-array-except-self" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="B14" r:id="rId122" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="A64" r:id="rId123" display="https://leetcode.com/problems/binary-tree-maximum-path-sum" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="B64" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="A72" r:id="rId125" display="https://leetcode.com/problems/continuous-subarray-sum" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="B72" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="A6" r:id="rId127" display="https://leetcode.com/problems/reverse-words-in-a-string-iii" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="B6" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="A33" r:id="rId129" display="https://leetcode.com/problems/add-strings" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="B33" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="A48" r:id="rId131" display="https://leetcode.com/problems/palindrome-linked-list" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="B48" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="A26" r:id="rId133" display="https://leetcode.com/problems/first-unique-character-in-a-string" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="B26" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="B18" r:id="rId135" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="B28" r:id="rId136" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="B57" r:id="rId137" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="B10" r:id="rId138" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="A28" r:id="rId119" display="https://leetcode.com/problems/partition-labels" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="B28" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="A33" r:id="rId121" display="https://leetcode.com/problems/product-of-array-except-self" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="B33" r:id="rId122" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="A71" r:id="rId123" display="https://leetcode.com/problems/binary-tree-maximum-path-sum" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="B71" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="A66" r:id="rId125" display="https://leetcode.com/problems/continuous-subarray-sum" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="B66" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="A4" r:id="rId127" display="https://leetcode.com/problems/reverse-words-in-a-string-iii" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="B4" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="A17" r:id="rId129" display="https://leetcode.com/problems/add-strings" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="B17" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="A22" r:id="rId131" display="https://leetcode.com/problems/palindrome-linked-list" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="B22" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="A15" r:id="rId133" display="https://leetcode.com/problems/first-unique-character-in-a-string" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="B15" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="B10" r:id="rId135" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="B39" r:id="rId136" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="B70" r:id="rId137" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="B7" r:id="rId138" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>